<commit_message>
data dictionary created, updated physical diagram
</commit_message>
<xml_diff>
--- a/final-project/data_dictionary.xlsx
+++ b/final-project/data_dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7320" firstSheet="30" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7320" firstSheet="29" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Mbrainz_Area_alias" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="73">
   <si>
     <t xml:space="preserve">Primary key </t>
   </si>
@@ -78,6 +78,201 @@
   </si>
   <si>
     <t>Explanations</t>
+  </si>
+  <si>
+    <t>gid</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>area_alias.csv</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>artist.csv</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>artist_alias.csv</t>
+  </si>
+  <si>
+    <t>gender.csv</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>place.csv</t>
+  </si>
+  <si>
+    <t>place_type.csv</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>language.csv</t>
+  </si>
+  <si>
+    <t>recording.csv</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>packaging</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>release.csv</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>catalog_number</t>
+  </si>
+  <si>
+    <t>release_label.csv</t>
+  </si>
+  <si>
+    <t>label_type.csv</t>
+  </si>
+  <si>
+    <t>release_packaging.csv</t>
+  </si>
+  <si>
+    <t>instrument_type.csv</t>
+  </si>
+  <si>
+    <t>begin_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>event.csv</t>
+  </si>
+  <si>
+    <t>series.csv</t>
+  </si>
+  <si>
+    <t>track.csv</t>
+  </si>
+  <si>
+    <t>ordering_type</t>
+  </si>
+  <si>
+    <t>varcchar(2000</t>
+  </si>
+  <si>
+    <t>ordering_type.csv</t>
+  </si>
+  <si>
+    <t>varchar (200)</t>
+  </si>
+  <si>
+    <t>series_type.csv</t>
+  </si>
+  <si>
+    <t>track_id</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>varchar (50)</t>
+  </si>
+  <si>
+    <t>lyrics.csv</t>
+  </si>
+  <si>
+    <t>tid</t>
+  </si>
+  <si>
+    <t>songs_summary.csv</t>
+  </si>
+  <si>
+    <t>words</t>
+  </si>
+  <si>
+    <t>words.csv</t>
+  </si>
+  <si>
+    <t>song</t>
+  </si>
+  <si>
+    <t>play_count</t>
+  </si>
+  <si>
+    <t>songs_popularity.csv</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>artist_id</t>
+  </si>
+  <si>
+    <t>artist_name</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>song_id</t>
+  </si>
+  <si>
+    <t>artists.csv</t>
+  </si>
+  <si>
+    <t>mbtag</t>
+  </si>
+  <si>
+    <t>artist_mbtag.csv</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>artist_term.csv</t>
   </si>
 </sst>
 </file>
@@ -414,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,6 +646,89 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -459,10 +737,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,6 +771,109 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -500,10 +881,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,6 +915,69 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -541,10 +985,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,6 +1019,69 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -582,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,6 +1123,69 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -623,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,6 +1227,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -664,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,6 +1291,52 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -705,16 +1344,18 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
@@ -735,6 +1376,129 @@
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -744,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -778,6 +1542,49 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -785,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -819,6 +1626,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -826,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -860,6 +1690,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -867,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,6 +1754,89 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -908,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,6 +1878,69 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -949,10 +1948,117 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,17 +2089,80 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1024,17 +2193,80 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,17 +2297,86 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1106,17 +2407,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1147,17 +2471,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1188,17 +2535,60 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1229,17 +2619,160 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1270,17 +2803,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1311,17 +2867,100 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,17 +2991,60 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1393,17 +3075,60 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1434,17 +3159,80 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1475,17 +3263,100 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,17 +3387,80 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1557,17 +3491,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1598,17 +3555,100 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1639,45 +3679,67 @@
         <v>7</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>